<commit_message>
Documentación de los códigos
</commit_message>
<xml_diff>
--- a/datos/personasdesdebdat.xlsx
+++ b/datos/personasdesdebdat.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="personas" r:id="rId5" sheetId="2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="54">
   <si>
     <t xml:space="preserve">nombre</t>
   </si>
@@ -35,6 +36,153 @@
   </si>
   <si>
     <t xml:space="preserve">género</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>apellidos</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>teléfono</t>
+  </si>
+  <si>
+    <t>género</t>
+  </si>
+  <si>
+    <t>OSCAR</t>
+  </si>
+  <si>
+    <t>MUÑOZ ORTIZ</t>
+  </si>
+  <si>
+    <t>omunort@mlb.bounce.ed10.net</t>
+  </si>
+  <si>
+    <t>684390051</t>
+  </si>
+  <si>
+    <t>MASCULINO</t>
+  </si>
+  <si>
+    <t>LIDIA</t>
+  </si>
+  <si>
+    <t>IGLESIAS MOYA</t>
+  </si>
+  <si>
+    <t>liglmoy@mail2saudi.com</t>
+  </si>
+  <si>
+    <t>717631732</t>
+  </si>
+  <si>
+    <t>FEMENINO</t>
+  </si>
+  <si>
+    <t>MOHAMED</t>
+  </si>
+  <si>
+    <t>HERRERA MARIN</t>
+  </si>
+  <si>
+    <t>mhermar@interburp.com</t>
+  </si>
+  <si>
+    <t>750292099</t>
+  </si>
+  <si>
+    <t>MARIA SOLEDAD</t>
+  </si>
+  <si>
+    <t>MORENO MORENO</t>
+  </si>
+  <si>
+    <t>mmormor@mail.ru</t>
+  </si>
+  <si>
+    <t>720699755</t>
+  </si>
+  <si>
+    <t>NEUTRO</t>
+  </si>
+  <si>
+    <t>RAMON</t>
+  </si>
+  <si>
+    <t>SANTOS SOTO</t>
+  </si>
+  <si>
+    <t>rsansot@outlook.it</t>
+  </si>
+  <si>
+    <t>622708296</t>
+  </si>
+  <si>
+    <t>MARIA ROSA</t>
+  </si>
+  <si>
+    <t>GARRIDO LEON</t>
+  </si>
+  <si>
+    <t>mgarleo@i.ua</t>
+  </si>
+  <si>
+    <t>701354268</t>
+  </si>
+  <si>
+    <t>PAU</t>
+  </si>
+  <si>
+    <t>PEÑA RODRIGUEZ</t>
+  </si>
+  <si>
+    <t>ppenrod@unforgettable.com</t>
+  </si>
+  <si>
+    <t>621041509</t>
+  </si>
+  <si>
+    <t>OTRO</t>
+  </si>
+  <si>
+    <t>FRANCISCO JOSE</t>
+  </si>
+  <si>
+    <t>CRESPO MARIN</t>
+  </si>
+  <si>
+    <t>fcremar@dfwatson.com</t>
+  </si>
+  <si>
+    <t>682207168</t>
+  </si>
+  <si>
+    <t>IRENE</t>
+  </si>
+  <si>
+    <t>GALLEGO SILVA</t>
+  </si>
+  <si>
+    <t>igalsil@digosnet.com</t>
+  </si>
+  <si>
+    <t>603398467</t>
+  </si>
+  <si>
+    <t>JOAQUIN</t>
+  </si>
+  <si>
+    <t>DOMINGO</t>
+  </si>
+  <si>
+    <t>jdomdom0901@g.educaan.es</t>
+  </si>
+  <si>
+    <t>640785273</t>
   </si>
 </sst>
 </file>
@@ -246,10 +394,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -269,6 +417,176 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -280,4 +598,204 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>